<commit_message>
edit in student controllers
</commit_message>
<xml_diff>
--- a/assets/adminAbsenceFiles/Database1.xlsx
+++ b/assets/adminAbsenceFiles/Database1.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -543,9 +543,56 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>200155</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Mohamed Elhefny</v>
+      </c>
+      <c r="D4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="H4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="L4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="M4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="N4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="O4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>